<commit_message>
Update Beta Testing Parts
</commit_message>
<xml_diff>
--- a/Experimental/StatsResultDf.xlsx
+++ b/Experimental/StatsResultDf.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -23,10 +23,10 @@
     <t>var</t>
   </si>
   <si>
+    <t>ptp</t>
+  </si>
+  <si>
     <t>mean</t>
-  </si>
-  <si>
-    <t>ptp</t>
   </si>
   <si>
     <t>std</t>
@@ -444,10 +444,10 @@
         <v>5.228185521309535</v>
       </c>
       <c r="D2" t="n">
+        <v>17.32899638</v>
+      </c>
+      <c r="E2" t="n">
         <v>14.98276364006452</v>
-      </c>
-      <c r="E2" t="n">
-        <v>17.32899638</v>
       </c>
       <c r="F2" t="n">
         <v>2.286522582724591</v>
@@ -464,10 +464,10 @@
         <v>9.196184370076589</v>
       </c>
       <c r="D3" t="n">
+        <v>23.07765895</v>
+      </c>
+      <c r="E3" t="n">
         <v>3.330604275470967</v>
-      </c>
-      <c r="E3" t="n">
-        <v>23.07765895</v>
       </c>
       <c r="F3" t="n">
         <v>3.0325211244238</v>
@@ -484,10 +484,10 @@
         <v>2.661431011356015</v>
       </c>
       <c r="D4" t="n">
+        <v>9.049359233000001</v>
+      </c>
+      <c r="E4" t="n">
         <v>3.610955847606452</v>
-      </c>
-      <c r="E4" t="n">
-        <v>9.049359233000001</v>
       </c>
       <c r="F4" t="n">
         <v>1.631389288721737</v>
@@ -504,10 +504,10 @@
         <v>3.417296632219134</v>
       </c>
       <c r="D5" t="n">
+        <v>9.59</v>
+      </c>
+      <c r="E5" t="n">
         <v>1.947420520670968</v>
-      </c>
-      <c r="E5" t="n">
-        <v>9.59</v>
       </c>
       <c r="F5" t="n">
         <v>1.848593149456942</v>
@@ -524,10 +524,10 @@
         <v>2.370211202975378</v>
       </c>
       <c r="D6" t="n">
+        <v>19.2</v>
+      </c>
+      <c r="E6" t="n">
         <v>0.2363086045419355</v>
-      </c>
-      <c r="E6" t="n">
-        <v>19.2</v>
       </c>
       <c r="F6" t="n">
         <v>1.539549025843405</v>
@@ -544,10 +544,10 @@
         <v>1.821717628826254</v>
       </c>
       <c r="D7" t="n">
+        <v>8.125834427000001</v>
+      </c>
+      <c r="E7" t="n">
         <v>3.628678976432258</v>
-      </c>
-      <c r="E7" t="n">
-        <v>8.125834427000001</v>
       </c>
       <c r="F7" t="n">
         <v>1.349710201793798</v>
@@ -564,10 +564,10 @@
         <v>0.1089255564679164</v>
       </c>
       <c r="D8" t="n">
+        <v>2.042</v>
+      </c>
+      <c r="E8" t="n">
         <v>0.3169630373096775</v>
-      </c>
-      <c r="E8" t="n">
-        <v>2.042</v>
       </c>
       <c r="F8" t="n">
         <v>0.3300387196495532</v>
@@ -584,10 +584,10 @@
         <v>99.52164917139636</v>
       </c>
       <c r="D9" t="n">
+        <v>48.34038846</v>
+      </c>
+      <c r="E9" t="n">
         <v>63.42915100670968</v>
-      </c>
-      <c r="E9" t="n">
-        <v>48.34038846</v>
       </c>
       <c r="F9" t="n">
         <v>9.9760537875152</v>
@@ -604,10 +604,10 @@
         <v>11.07863974613074</v>
       </c>
       <c r="D10" t="n">
+        <v>14.8266616</v>
+      </c>
+      <c r="E10" t="n">
         <v>5.519617054748387</v>
-      </c>
-      <c r="E10" t="n">
-        <v>14.8266616</v>
       </c>
       <c r="F10" t="n">
         <v>3.328459064812236</v>
@@ -624,10 +624,10 @@
         <v>0.307774247695323</v>
       </c>
       <c r="D11" t="n">
+        <v>2.68</v>
+      </c>
+      <c r="E11" t="n">
         <v>0.839078381051613</v>
-      </c>
-      <c r="E11" t="n">
-        <v>2.68</v>
       </c>
       <c r="F11" t="n">
         <v>0.5547740510291762</v>

</xml_diff>